<commit_message>
test search and add to watchlist added
</commit_message>
<xml_diff>
--- a/com.investing/src/test/resources/test_data.xlsx
+++ b/com.investing/src/test/resources/test_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadou\IdeaProjects\SeleniumBootcamp\com.investing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4960305-ABDE-4D98-8726-F061BC4CCB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243F33CD-6004-4088-A5FA-1E15FAE5EF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E7B6A4B2-679E-4BF3-90F5-28D487287812}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E7B6A4B2-679E-4BF3-90F5-28D487287812}"/>
   </bookViews>
   <sheets>
     <sheet name="doLogIn" sheetId="1" r:id="rId1"/>
+    <sheet name="doSearch" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Email</t>
   </si>
@@ -58,6 +59,21 @@
   </si>
   <si>
     <t>Serpent9999+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Term </t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Etherium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bitcoin </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonds </t>
   </si>
 </sst>
 </file>
@@ -428,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29AF4ED9-AFE8-4409-89FF-574866C7DEC0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -479,4 +495,47 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8CF7EE3-2724-4232-B54D-1DC59D9AB984}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>